<commit_message>
Added the environment properties file and updated pom.xml for maven lifecycle & profile
</commit_message>
<xml_diff>
--- a/RedBusAutomation/src/test/resources/TestData.xlsx
+++ b/RedBusAutomation/src/test/resources/TestData.xlsx
@@ -1,22 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{6A84F67A-D22A-4EB1-AC71-405587ED2334}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2472" windowWidth="12816" windowHeight="5376"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="12840" windowHeight="8835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>performLogin</t>
   </si>
@@ -27,14 +29,23 @@
     <t>indore</t>
   </si>
   <si>
-    <t>07-Jul-2020</t>
+    <t>Indore</t>
+  </si>
+  <si>
+    <t>bhopal</t>
+  </si>
+  <si>
+    <t>07-Apr-2021</t>
+  </si>
+  <si>
+    <t>07-Mar-2021</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -72,6 +83,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -118,7 +137,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -150,9 +169,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -184,6 +221,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -359,31 +414,42 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.88671875" style="1"/>
+    <col min="4" max="4" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D2" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
         <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -393,24 +459,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Adding the test data
</commit_message>
<xml_diff>
--- a/RedBusAutomation/src/test/resources/TestData.xlsx
+++ b/RedBusAutomation/src/test/resources/TestData.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{6A84F67A-D22A-4EB1-AC71-405587ED2334}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{78E7BA83-DA14-4EE1-B4C4-95229FC9AACE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="12840" windowHeight="8835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="12870" windowHeight="11820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>performLogin</t>
   </si>
@@ -39,6 +39,15 @@
   </si>
   <si>
     <t>07-Mar-2021</t>
+  </si>
+  <si>
+    <t>Pune</t>
+  </si>
+  <si>
+    <t>Hyderabad</t>
+  </si>
+  <si>
+    <t>07-Jun-2021</t>
   </si>
 </sst>
 </file>
@@ -415,13 +424,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
@@ -450,6 +462,17 @@
       </c>
       <c r="D3" s="1" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Removed the changes in excel
</commit_message>
<xml_diff>
--- a/RedBusAutomation/src/test/resources/TestData.xlsx
+++ b/RedBusAutomation/src/test/resources/TestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{78E7BA83-DA14-4EE1-B4C4-95229FC9AACE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{0F965EE8-B4BA-4D3C-A4D8-9CF2DAAA682E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2340" windowWidth="12870" windowHeight="11820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="12900" windowHeight="11820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>performLogin</t>
   </si>
@@ -39,15 +39,6 @@
   </si>
   <si>
     <t>07-Mar-2021</t>
-  </si>
-  <si>
-    <t>Pune</t>
-  </si>
-  <si>
-    <t>Hyderabad</t>
-  </si>
-  <si>
-    <t>07-Jun-2021</t>
   </si>
 </sst>
 </file>
@@ -426,8 +417,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -464,17 +455,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added test in excel
</commit_message>
<xml_diff>
--- a/RedBusAutomation/src/test/resources/TestData.xlsx
+++ b/RedBusAutomation/src/test/resources/TestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{0F965EE8-B4BA-4D3C-A4D8-9CF2DAAA682E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{0EF3239F-8DC2-49DA-BD15-8771738AB5CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="1950" windowWidth="12900" windowHeight="11820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="12930" windowHeight="11820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="7">
   <si>
     <t>performLogin</t>
   </si>
@@ -455,7 +455,17 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>